<commit_message>
Updated CloseAllApplications, GetTransactionData, InitAllApplications, and KillAllProcess xaml files
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\OneDrive\Documents\UiPath\REF_GenerateYearlyReport\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA9724C-78BD-43E5-A7F1-AE3C520357E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF08A044-71C8-463D-AEF0-1E322ABE0ED8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -560,7 +560,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2819,7 +2819,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Added System1_DownloadMonthlyReport, System1_GetClientDetails , System1_ReturnToDashboard xaml files
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\OneDrive\Documents\UiPath\REF_GenerateYearlyReport\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\OneDrive\Documents\UiPath Advance\REF_GenerateYearlyReport\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF08A044-71C8-463D-AEF0-1E322ABE0ED8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38CB642-5527-4375-8EC3-4FD570D00A4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -175,6 +175,15 @@
   </si>
   <si>
     <t>REF_YearlyReportQueues</t>
+  </si>
+  <si>
+    <t>ReportDirPath</t>
+  </si>
+  <si>
+    <t>C:\Users\Charlie\OneDrive\Documents\UiPath Advance\REF_GenerateYearlyReport\Data\Output</t>
+  </si>
+  <si>
+    <t>Path to download reports</t>
   </si>
 </sst>
 </file>
@@ -560,13 +569,13 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="2" max="2" width="89.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -655,7 +664,17 @@
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Updated the process.xaml file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\OneDrive\Documents\UiPath Advance\REF_GenerateYearlyReport\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlie\OneDrive\Documents\UiPath Advance\REF_GenerateYearlyReport_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38CB642-5527-4375-8EC3-4FD570D00A4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB5F9C8-056B-423E-97C8-DF0C525DD26F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -156,9 +156,6 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>REF_GenerateYearlyReport</t>
-  </si>
-  <si>
     <t>ACME_LoginCredential</t>
   </si>
   <si>
@@ -180,10 +177,49 @@
     <t>ReportDirPath</t>
   </si>
   <si>
-    <t>C:\Users\Charlie\OneDrive\Documents\UiPath Advance\REF_GenerateYearlyReport\Data\Output</t>
-  </si>
-  <si>
     <t>Path to download reports</t>
+  </si>
+  <si>
+    <t>REF_GenerateYearlyReport-Performer</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/work-items</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/reports/download</t>
+  </si>
+  <si>
+    <t>UploadYearlyReport_URL</t>
+  </si>
+  <si>
+    <t>WorkItems_URL</t>
+  </si>
+  <si>
+    <t>DownloadMonthlyReport_URL</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/reports/upload</t>
+  </si>
+  <si>
+    <t>Comment Status</t>
+  </si>
+  <si>
+    <t>Download Monthly Report URL</t>
+  </si>
+  <si>
+    <t>Upload Yearly Report URL</t>
+  </si>
+  <si>
+    <t>Work Items url</t>
+  </si>
+  <si>
+    <t>C:\Users\Charlie\OneDrive\Documents\UiPath Advance\REF_GenerateYearlyReport_Performer\Data\Reports\</t>
   </si>
 </sst>
 </file>
@@ -569,13 +605,13 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="89.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="101" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -619,7 +655,7 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -630,7 +666,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>31</v>
@@ -642,7 +678,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -654,32 +690,72 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" t="s">
         <v>50</v>
-      </c>
-      <c r="B9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -2887,16 +2963,16 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>